<commit_message>
working transient landuses with volume outputs per day
</commit_message>
<xml_diff>
--- a/Checks.xlsx
+++ b/Checks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\openwaternetwork\swatplus_transient_lu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62693AE-FF23-4CB5-BEEB-8F4B244C88D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB86A475-4EC8-45F9-B8BD-61F02718A3F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30495" yWindow="2745" windowWidth="25695" windowHeight="11385" xr2:uid="{5510C489-6ED1-448C-92B0-91435F6F8756}"/>
   </bookViews>
@@ -5577,7 +5577,7 @@
   <dimension ref="A1:S229"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:M3"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>